<commit_message>
Update T&D loss percentage
</commit_message>
<xml_diff>
--- a/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
+++ b/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\Texas\InputData\elec\BTaDLP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-texas\InputData\elec\BTaDLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B18E8A4-4C6B-4B4C-A604-932D442712C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49410" yWindow="855" windowWidth="17595" windowHeight="15765" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49410" yWindow="855" windowWidth="17595" windowHeight="15765"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="MER 7.1" sheetId="6" r:id="rId2"/>
     <sheet name="Calculations" sheetId="4" r:id="rId3"/>
     <sheet name="Texas Notes" sheetId="7" r:id="rId4"/>
-    <sheet name="BTaDLP" sheetId="2" r:id="rId5"/>
+    <sheet name="WISdom results" sheetId="8" r:id="rId5"/>
+    <sheet name="BTaDLP" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="79">
   <si>
     <t>Source:</t>
   </si>
@@ -297,12 +297,15 @@
   </si>
   <si>
     <t>We'll just use the same trend as the national data--which is flat (i.e. losses don't get any better throough 2050)</t>
+  </si>
+  <si>
+    <t>Average transmission losses across all TX regions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -446,7 +449,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -493,11 +496,14 @@
     <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -675,6 +681,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1301,6 +1308,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1308,7 +1316,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2057,23 +2064,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2109,23 +2099,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2301,10 +2274,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -2360,7 +2333,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" location="electricity" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1" location="electricity"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -2368,7 +2341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5038,7 +5011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5360,10 +5333,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97F9CBF-B5D6-4E97-84A1-BE76069BA22F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -6191,14 +6164,40 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="25.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1">
+        <v>0.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2:AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6325,147 +6324,148 @@
         <v>33</v>
       </c>
       <c r="B2" s="4">
-        <f>'Texas Notes'!B11</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="C2" s="4">
-        <f t="array" ref="C2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!C1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="D2" s="4">
-        <f t="array" ref="D2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!D1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="E2" s="4">
-        <f t="array" ref="E2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!E1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="F2" s="4">
-        <f t="array" ref="F2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!F1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="G2" s="4">
-        <f t="array" ref="G2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!G1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="H2" s="4">
-        <f t="array" ref="H2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!H1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="I2" s="4">
-        <f t="array" ref="I2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!I1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="J2" s="4">
-        <f t="array" ref="J2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!J1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="K2" s="4">
-        <f t="array" ref="K2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!K1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="L2" s="4">
-        <f t="array" ref="L2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!L1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="M2" s="4">
-        <f t="array" ref="M2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!M1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="N2" s="4">
-        <f t="array" ref="N2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!N1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="O2" s="4">
-        <f t="array" ref="O2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!O1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="P2" s="4">
-        <f t="array" ref="P2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!P1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="Q2" s="4">
-        <f t="array" ref="Q2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!Q1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="R2" s="4">
-        <f t="array" ref="R2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!R1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="S2" s="4">
-        <f t="array" ref="S2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!S1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="T2" s="4">
-        <f t="array" ref="T2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!T1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="U2" s="4">
-        <f t="array" ref="U2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!U1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="V2" s="4">
-        <f t="array" ref="V2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!V1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="W2" s="4">
-        <f t="array" ref="W2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!W1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="X2" s="4">
-        <f t="array" ref="X2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!X1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="Y2" s="4">
-        <f t="array" ref="Y2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!Y1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="Z2" s="4">
-        <f t="array" ref="Z2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!Z1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AA2" s="4">
-        <f t="array" ref="AA2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AA1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AB2" s="4">
-        <f t="array" ref="AB2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AB1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AC2" s="4">
-        <f t="array" ref="AC2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AC1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AD2" s="4">
-        <f t="array" ref="AD2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AD1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AE2" s="4">
-        <f t="array" ref="AE2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AE1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AF2" s="4">
-        <f t="array" ref="AF2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AF1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AG2" s="4">
-        <f t="array" ref="AG2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AG1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AH2" s="4">
-        <f t="array" ref="AH2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AH1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AI2" s="4">
-        <f t="array" ref="AI2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AI1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AJ2" s="4">
-        <f t="array" ref="AJ2">TREND('Texas Notes'!$B$32:$C$32,'Texas Notes'!$B$31:$C$31,BTaDLP!AJ1)</f>
-        <v>5.0668929575420463E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
       <c r="AK2" s="4">
-        <v>5.0999999999999997E-2</v>
+        <f>'WISdom results'!$B$1</f>
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>